<commit_message>
Ajouter un test pour > 1 caractère particulié
</commit_message>
<xml_diff>
--- a/test/sample_sheet_index_not_ATCG_format.xlsx
+++ b/test/sample_sheet_index_not_ATCG_format.xlsx
@@ -1123,7 +1123,7 @@
     <t xml:space="preserve">SSIJ125</t>
   </si>
   <si>
-    <t xml:space="preserve">CGTACACTGG</t>
+    <t xml:space="preserve">CGTACACTGGY</t>
   </si>
   <si>
     <t xml:space="preserve">GKRH1405</t>
@@ -2009,9 +2009,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>741600</xdr:colOff>
+      <xdr:colOff>741240</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:rowOff>52200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2025,7 +2025,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5542200" y="50760"/>
-          <a:ext cx="10944000" cy="1017720"/>
+          <a:ext cx="10943640" cy="1017360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2048,10 +2048,10 @@
   <dimension ref="A1:M118"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H77" activeCellId="0" sqref="H77"/>
+      <selection pane="topLeft" activeCell="H92" activeCellId="0" sqref="H92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.53125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18"/>

</xml_diff>